<commit_message>
!ref make me angy
</commit_message>
<xml_diff>
--- a/backend/temp.xlsx
+++ b/backend/temp.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Worksheet 3" sheetId="4" r:id="rId4"/>
     <sheet name="Worksheet 4" sheetId="5" r:id="rId5"/>
     <sheet name="Worksheet 5" sheetId="6" r:id="rId6"/>
+    <sheet name="test1" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -563,7 +564,7 @@
         <v>191039</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v/>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="str">
         <v/>
@@ -574,7 +575,7 @@
     </row>
     <row r="15">
       <c r="C15" s="1" t="str">
-        <v>/33</v>
+        <v>/</v>
       </c>
       <c r="D15" s="1" t="str">
         <v>/</v>
@@ -588,7 +589,7 @@
         <v>201002</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D19" s="1" t="str">
         <v/>
@@ -599,7 +600,7 @@
     </row>
     <row r="20">
       <c r="C20" s="1" t="str">
-        <v>/96</v>
+        <v>/</v>
       </c>
       <c r="D20" s="1" t="str">
         <v>/</v>
@@ -613,7 +614,7 @@
         <v>201004</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D24" s="1" t="str">
         <v/>
@@ -624,7 +625,7 @@
     </row>
     <row r="25">
       <c r="C25" s="1" t="str">
-        <v>/78</v>
+        <v>/</v>
       </c>
       <c r="D25" s="1" t="str">
         <v>/</v>
@@ -638,7 +639,7 @@
         <v>201006</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D29" s="1" t="str">
         <v/>
@@ -649,7 +650,7 @@
     </row>
     <row r="30">
       <c r="C30" s="1" t="str">
-        <v>/65</v>
+        <v>/</v>
       </c>
       <c r="D30" s="1" t="str">
         <v>/</v>
@@ -663,7 +664,7 @@
         <v>201009</v>
       </c>
       <c r="C34" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D34" s="1" t="str">
         <v/>
@@ -674,7 +675,7 @@
     </row>
     <row r="35">
       <c r="C35" s="1" t="str">
-        <v>/86</v>
+        <v>/</v>
       </c>
       <c r="D35" s="1" t="str">
         <v>/</v>
@@ -688,7 +689,7 @@
         <v>201019</v>
       </c>
       <c r="C39" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D39" s="1" t="str">
         <v/>
@@ -699,7 +700,7 @@
     </row>
     <row r="40">
       <c r="C40" s="1" t="str">
-        <v>/12</v>
+        <v>/</v>
       </c>
       <c r="D40" s="1" t="str">
         <v>/</v>
@@ -713,7 +714,7 @@
         <v>201022</v>
       </c>
       <c r="C44" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D44" s="1" t="str">
         <v/>
@@ -724,7 +725,7 @@
     </row>
     <row r="45">
       <c r="C45" s="1" t="str">
-        <v>/78</v>
+        <v>/</v>
       </c>
       <c r="D45" s="1" t="str">
         <v>/</v>
@@ -738,7 +739,7 @@
         <v>201024</v>
       </c>
       <c r="C49" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D49" s="1" t="str">
         <v/>
@@ -749,7 +750,7 @@
     </row>
     <row r="50">
       <c r="C50" s="1" t="str">
-        <v>/76</v>
+        <v>/</v>
       </c>
       <c r="D50" s="1" t="str">
         <v>/</v>
@@ -763,7 +764,7 @@
         <v>201026</v>
       </c>
       <c r="C54" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D54" s="1" t="str">
         <v/>
@@ -774,7 +775,7 @@
     </row>
     <row r="55">
       <c r="C55" s="1" t="str">
-        <v>/76</v>
+        <v>/</v>
       </c>
       <c r="D55" s="1" t="str">
         <v>/</v>
@@ -788,7 +789,7 @@
         <v>201029</v>
       </c>
       <c r="C59" s="1" t="str">
-        <v/>
+        <v>-8</v>
       </c>
       <c r="D59" s="1" t="str">
         <v/>
@@ -799,7 +800,7 @@
     </row>
     <row r="60">
       <c r="C60" s="1" t="str">
-        <v>/56</v>
+        <v>/</v>
       </c>
       <c r="D60" s="1" t="str">
         <v>/</v>
@@ -3152,4 +3153,431 @@
     <ignoredError numberStoredAsText="1" sqref="A1:L24"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="str">
+        <v>ST. FRANCIS INSTITUTE OF TECHNOLOGY</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="str">
+        <v xml:space="preserve"> UNIVERSITY OF MUMBAI</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>COURSE I:ETS401     :</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>COURSE II:ETC402     :</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <v>COURSE III:ETC403     :</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>COURSE IV:ETC404     :</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <v>COURSE V:ETC405     :</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <v>COURSE VI:ETC406     :</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
+        <v>COURSE VII:ETL401     :</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <v>COURSE VIII:ETL402     :</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <v>COURSE IX:ETL403     :</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="1" t="str">
+        <v>&lt;------Course I------&gt;</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <v>&lt;------Course II------&gt;</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <v>&lt;------Course III------&gt;</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <v>&lt;------Course IV------&gt;</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="str">
+        <v>THEORY</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <v>80/32   20/8   100 C G GP C*GP</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <v>80/32   20/8   100 C G GP C*GP</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <v>80/32   20/8   100 C G GP C*GP</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <v>80/32   20/8   100 C G GP C*GP</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="str">
+        <v>TERMWORK/ORAL</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <v>25/10   C G GP C*GP</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="1" t="str">
+        <v>&lt;------Course V------&gt;</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <v>&lt;------Course VI------&gt;</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <v>&lt;------Course VII------&gt;</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <v>&lt;------Course VIII------&gt;</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <v>&lt;------Course IX------&gt;</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="str">
+        <v>THEORY</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <v>80/32   20/8   100 C G GP C*GP</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <v>80/32   20/8   100 C G GP C*GP</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="1" t="str">
+        <v>TERMWORK/ORAL</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v>25/10   C G GP C*GP</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <v>25/10  25/10    50 C G GP C*GP</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <v>25/10  25/10    50 C G GP C*GP</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <v>25/10  25/10    50 C G GP C*GP</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <v>∑C</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <v>∑CG</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <v>GPA</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="str">
+        <v>191039</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E14" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="str">
+        <v>201002</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E19" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <v>201004</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E24" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="str">
+        <v>201006</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E29" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="str">
+        <v>201009</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E34" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="str">
+        <v>201019</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E39" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="str">
+        <v>201022</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E44" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="str">
+        <v>201024</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E49" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="str">
+        <v>201026</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E54" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="str">
+        <v>201029</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <v>-8</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E59" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <v>/</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <v>/</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L62"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>